<commit_message>
adding styles to excel
</commit_message>
<xml_diff>
--- a/src/tasks/syncs/portalCheck/excelTask/template.xlsx
+++ b/src/tasks/syncs/portalCheck/excelTask/template.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Documents\GitHub\yumetetsu-cron\src\tasks\syncs\portalCheck\excelTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A04FFE-96DB-478B-95D1-6575BE2444B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6014BCD-0676-4F8E-90C7-74EE703B6C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99EF1909-4568-42E4-9596-BB46F4289826}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{509F8091-917D-4394-9838-02BB04CB4F57}"/>
   </bookViews>
   <sheets>
-    <sheet name="中古マンション" sheetId="10" r:id="rId1"/>
-    <sheet name="中古戸建" sheetId="11" r:id="rId2"/>
-    <sheet name="土地" sheetId="12" r:id="rId3"/>
+    <sheet name="中古マンション" sheetId="1" r:id="rId1"/>
+    <sheet name="中古戸建" sheetId="3" r:id="rId2"/>
+    <sheet name="土地" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
   <si>
     <t>物件名</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>資料有り</t>
-  </si>
-  <si>
-    <t>URL_ハイパーリンク</t>
   </si>
   <si>
     <t>掲載企業</t>
@@ -110,6 +107,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="游ゴシック"/>
@@ -161,15 +159,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,25 +478,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:O1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86646669-F0E6-4365-8175-538F5583845A}">
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="30.625" customWidth="1"/>
     <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,70 +508,131 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62651B4-EF79-4341-800F-A4A5479D203D}">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="30.625" customWidth="1"/>
+    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C102DB46-EBB5-4852-A502-0199E5FAA23F}">
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="34.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.625" customWidth="1"/>
+    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,119 +643,42 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="45.375" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="58.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added format to excel
</commit_message>
<xml_diff>
--- a/src/tasks/syncs/portalCheck/excelTask/template.xlsx
+++ b/src/tasks/syncs/portalCheck/excelTask/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Documents\GitHub\yumetetsu-cron\src\tasks\syncs\portalCheck\excelTask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\yumetetsu-cron\src\tasks\syncs\portalCheck\excelTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6014BCD-0676-4F8E-90C7-74EE703B6C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A120F7-1B03-4724-BFC9-D50B53ADB387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{509F8091-917D-4394-9838-02BB04CB4F57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{509F8091-917D-4394-9838-02BB04CB4F57}"/>
   </bookViews>
   <sheets>
     <sheet name="中古マンション" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>物件名</t>
   </si>
@@ -46,12 +46,6 @@
     <t>所在地</t>
   </si>
   <si>
-    <t>専有面積</t>
-  </si>
-  <si>
-    <t>DOネットの管理有無</t>
-  </si>
-  <si>
     <t>物件番号</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
   </si>
   <si>
     <t>資料有り</t>
-  </si>
-  <si>
-    <t>掲載企業</t>
   </si>
   <si>
     <t>掲載企業TEL</t>
@@ -85,12 +76,42 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>DO管理有無</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>専有面積</t>
+    <rPh sb="0" eb="2">
+      <t>センユウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>メンセキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>専有面積</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(リンク)掲載企業</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（リンク）掲載企業</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（リンク）掲載企業</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +136,24 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -130,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -139,16 +178,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -159,15 +228,34 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -183,7 +271,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -481,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86646669-F0E6-4365-8175-538F5583845A}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -495,48 +583,48 @@
     <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -550,7 +638,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -563,48 +651,48 @@
     <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -618,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C102DB46-EBB5-4852-A502-0199E5FAA23F}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -632,48 +720,48 @@
     <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>